<commit_message>
fixed date on AERA training
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Desktop/trial-cv/_cv_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BE05F1-FBFC-874A-A0F1-8D5CCC2B982D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87AD020-5A08-F44A-9DBA-C22BC1D3D560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t>workshop-delivered</t>
   </si>
   <si>
-    <t>April, 2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">Developing transparent and reproducible research with R </t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>Maximizing pilot phase measures to inform quality improvement: Using a sequential mixed methods design with interrupted time series to examine feasibility, uptake, and drivers of an evidence based practice in part c/early intervention systems</t>
+  </si>
+  <si>
+    <t>April, 2019</t>
   </si>
 </sst>
 </file>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D849796-8D2F-2144-8637-FA01837A8DE5}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,7 +880,7 @@
         <v>2018</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>42</v>
@@ -889,7 +889,7 @@
         <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -911,13 +911,13 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -925,147 +925,147 @@
         <v>46</v>
       </c>
       <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" t="s">
         <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30">
         <v>2017</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31">
         <v>2009</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" t="s">
         <v>72</v>
-      </c>
-      <c r="F31" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34">
         <v>2018</v>
@@ -1074,13 +1074,13 @@
         <v>2019</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
       </c>
       <c r="F34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added social data science network membership to service
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87AD020-5A08-F44A-9DBA-C22BC1D3D560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B10A5A-8AAE-4341-AE46-C82D7FA96DC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
   <si>
     <t>type</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>April, 2019</t>
+  </si>
+  <si>
+    <t>Core Member (two-year appointment): Social Systems Data Science Network</t>
   </si>
 </sst>
 </file>
@@ -625,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D849796-8D2F-2144-8637-FA01837A8DE5}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -876,48 +879,51 @@
       <c r="A15" t="s">
         <v>41</v>
       </c>
-      <c r="B15">
-        <v>2018</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
-      </c>
-      <c r="G15" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B16">
+        <v>2018</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -925,21 +931,27 @@
         <v>46</v>
       </c>
       <c r="C18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -947,7 +959,7 @@
         <v>63</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -955,7 +967,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -963,7 +975,7 @@
         <v>63</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -971,7 +983,7 @@
         <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -979,7 +991,7 @@
         <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -987,7 +999,7 @@
         <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -995,7 +1007,7 @@
         <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1003,7 +1015,7 @@
         <v>63</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1011,7 +1023,7 @@
         <v>63</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1019,18 +1031,15 @@
         <v>63</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30">
-        <v>2017</v>
+        <v>63</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1038,21 +1047,24 @@
         <v>64</v>
       </c>
       <c r="C31">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="C32">
+        <v>2009</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="F32" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1060,26 +1072,34 @@
         <v>66</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>73</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>2018</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>2019</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>11</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added volume/pages to SESI pub. Added DVS to
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B10A5A-8AAE-4341-AE46-C82D7FA96DC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93EDAB3-5CE2-034E-B2D5-9CD428624B61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="80">
   <si>
     <t>type</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>Core Member (two-year appointment): Social Systems Data Science Network</t>
+  </si>
+  <si>
+    <t>Data Visualization Society</t>
+  </si>
+  <si>
+    <t>https://www.datavisualizationsociety.com</t>
   </si>
 </sst>
 </file>
@@ -628,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D849796-8D2F-2144-8637-FA01837A8DE5}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1067,7 +1073,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -1083,23 +1089,34 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>73</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>2018</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>2019</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>11</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added deep learning workshop
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93EDAB3-5CE2-034E-B2D5-9CD428624B61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC60679-578F-6441-B07C-A453A20E5A55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
+    <workbookView xWindow="25260" yWindow="1760" windowWidth="33600" windowHeight="20040" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
   <sheets>
     <sheet name="cv_entries" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
   <si>
     <t>type</t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>https://www.datavisualizationsociety.com</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>*Deep Learning with Keras and TensorFlow in R*</t>
+  </si>
+  <si>
+    <t>Two-day workshop lead by Dr. Brad Boehmke</t>
   </si>
 </sst>
 </file>
@@ -634,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D849796-8D2F-2144-8637-FA01837A8DE5}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,264 +830,271 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>80</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>31</v>
+      <c r="C13" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="3">
-        <v>2016</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>33</v>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>70</v>
+        <v>26</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3">
+        <v>2016</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="B16">
-        <v>2018</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
       </c>
-      <c r="G16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B17">
+        <v>2018</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
       <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>63</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>63</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>63</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31">
-        <v>2017</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>64</v>
       </c>
       <c r="C32">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="C33">
+        <v>2009</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="F33" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1086,7 +1102,7 @@
         <v>66</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1094,29 +1110,37 @@
         <v>66</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G35" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>73</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>2018</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>2019</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>11</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added COE quant committee service
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A38169E-8D02-794D-80BC-28D0C8FEA1B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9615D83-669D-0D4E-BEA7-66ED93DDE8E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25260" yWindow="1760" windowWidth="33600" windowHeight="20040" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
   <si>
     <t>type</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Two-day workshop lead by Dr. Bradley Boehmke</t>
+  </si>
+  <si>
+    <t>COE Quantitative Curriculum Review Committee Member</t>
   </si>
 </sst>
 </file>
@@ -640,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D849796-8D2F-2144-8637-FA01837A8DE5}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,28 +946,31 @@
       <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B18">
+        <v>2019</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -972,21 +978,27 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -994,7 +1006,7 @@
         <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1002,7 +1014,7 @@
         <v>62</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1010,7 +1022,7 @@
         <v>62</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1018,7 +1030,7 @@
         <v>62</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1026,7 +1038,7 @@
         <v>62</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1034,7 +1046,7 @@
         <v>62</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1042,7 +1054,7 @@
         <v>62</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1050,7 +1062,7 @@
         <v>62</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1058,18 +1070,15 @@
         <v>62</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31">
-        <v>2017</v>
+        <v>62</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1077,21 +1086,24 @@
         <v>63</v>
       </c>
       <c r="C32">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="C33">
+        <v>2009</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="F33" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1099,7 +1111,7 @@
         <v>65</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1107,29 +1119,37 @@
         <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G35" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>72</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>2018</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>2019</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>11</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add data science fellow
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E44175F-71BC-4F4E-BFB6-15AFB085B8B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E37F679-DDEE-9644-9208-2DB9E77AF3D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25260" yWindow="1760" windowWidth="33600" windowHeight="20040" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="84">
   <si>
     <t>type</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Awarded for outstanding Master's degree Terminal Project, University of Oregon College of Education</t>
+  </si>
+  <si>
+    <t>*Data Science Fellow*: College of Education, University of Oregon</t>
   </si>
 </sst>
 </file>
@@ -643,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D849796-8D2F-2144-8637-FA01837A8DE5}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,15 +1084,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>63</v>
       </c>
       <c r="C32">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1097,21 +1100,24 @@
         <v>63</v>
       </c>
       <c r="C33">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="C34">
+        <v>2009</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="F34" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1119,7 +1125,7 @@
         <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1127,29 +1133,37 @@
         <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G36" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>2018</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>2019</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>11</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>